<commit_message>
08-02-2024 excel upload fixes
</commit_message>
<xml_diff>
--- a/userfiles/employee/Employee-Management-Template.xlsx
+++ b/userfiles/employee/Employee-Management-Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="262">
   <si>
     <t>username</t>
   </si>
@@ -784,9 +784,6 @@
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>employee_type</t>
-  </si>
-  <si>
     <t>gender (male,female)</t>
   </si>
   <si>
@@ -803,6 +800,12 @@
   </si>
   <si>
     <t>joined date</t>
+  </si>
+  <si>
+    <t>role (ADMIN, General Workers)</t>
+  </si>
+  <si>
+    <t>employee_type(domestic,foreign)</t>
   </si>
 </sst>
 </file>
@@ -1197,17 +1200,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="41.7109375" customWidth="1"/>
+    <col min="15" max="15" width="34" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1222,8 +1229,9 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1249,41 +1257,45 @@
         <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="N2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" location="'References for Country Name'!A1" display="country"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
21-02-2023 after mdec meeting
</commit_message>
<xml_diff>
--- a/userfiles/employee/Employee-Management-Template.xlsx
+++ b/userfiles/employee/Employee-Management-Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="265">
   <si>
     <t>username</t>
   </si>
@@ -806,6 +806,15 @@
   </si>
   <si>
     <t>employee_type(domestic,foreign)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bank name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bank account number</t>
+  </si>
+  <si>
+    <t>ic number</t>
   </si>
 </sst>
 </file>
@@ -1200,19 +1209,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="41.7109375" customWidth="1"/>
-    <col min="15" max="15" width="34" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" customWidth="1"/>
+    <col min="16" max="16" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>258</v>
       </c>
@@ -1230,8 +1239,11 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1242,57 +1254,69 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G2" location="'References for Country Name'!A1" display="country"/>
+    <hyperlink ref="H2" location="'References for Country Name'!A1" display="country"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>